<commit_message>
fixed an issue with the cocktail number and the cocktaillist
</commit_message>
<xml_diff>
--- a/TimePlan.xlsx
+++ b/TimePlan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Erweiterung</t>
   </si>
@@ -31,9 +31,6 @@
   </si>
   <si>
     <t>Feste Rezeptnummer</t>
-  </si>
-  <si>
-    <t>0.5h</t>
   </si>
 </sst>
 </file>
@@ -370,7 +367,7 @@
   <dimension ref="A1:C83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -393,8 +390,8 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
+      <c r="B2" s="1">
+        <v>2</v>
       </c>
       <c r="C2" s="1"/>
     </row>

</xml_diff>

<commit_message>
added 2nd User-Story functionality
</commit_message>
<xml_diff>
--- a/TimePlan.xlsx
+++ b/TimePlan.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B8B137-00BD-B148-A1DB-FC8AE5682A15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Erweiterung</t>
   </si>
@@ -32,11 +33,14 @@
   <si>
     <t>Feste Rezeptnummer</t>
   </si>
+  <si>
+    <t>Warnungen</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -363,19 +367,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="1" max="1" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -386,416 +390,424 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1">
         <v>2</v>
       </c>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>

</xml_diff>

<commit_message>
working on printAmount for double ingredients, not working correctly i think, please check again
</commit_message>
<xml_diff>
--- a/TimePlan.xlsx
+++ b/TimePlan.xlsx
@@ -1,26 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B8B137-00BD-B148-A1DB-FC8AE5682A15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Erweiterung</t>
   </si>
@@ -31,34 +24,42 @@
     <t>Maciej</t>
   </si>
   <si>
-    <t>Feste Rezeptnummer</t>
+    <t>Gesamt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feste Rezeptnummer</t>
   </si>
   <si>
     <t>Warnungen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nicht-mischbare löschen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1">
     <font>
+      <name val="Calibri"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
+    <fill/>
+    <fill/>
   </fills>
-  <borders count="2">
+  <borders count="3">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -83,30 +84,306 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+  <cellXfs count="3">
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="2" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="2" numFmtId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Angsana New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Cordia New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -148,74 +425,14 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:latin typeface="Calibri Light"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -223,7 +440,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -249,7 +466,7 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -301,16 +518,28 @@
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -326,7 +555,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -357,29 +586,22 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C83"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0" zoomScale="100">
+      <selection activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="30.00390625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -389,10 +611,13 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1">
         <v>2</v>
@@ -401,9 +626,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1">
         <v>4</v>
@@ -412,407 +637,440 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <f>SUM(B4:C4)</f>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <f>SUM(B5:C5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E6">
+        <f>SUM(B6:C6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <f>SUM(B7:C7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E8">
+        <f>SUM(B8:C8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E9">
+        <f>SUM(B9:C9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="62">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="63">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="64">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="65">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="66">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="67">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="68">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="69">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="70">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="71">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="72">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="73">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="74">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="75">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="76">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="77">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="78">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="79">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="80">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="81">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="82">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="83">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <printOptions headings="0" gridLines="0" gridLinesSet="0"/>
+  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="-1" fitToHeight="0" fitToWidth="0" horizontalDpi="600" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="600"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
map scheint mit dem iterator ein problem zu haben. find findet korrekte werte, for-schleife gibt 1.0e+6 aus
</commit_message>
<xml_diff>
--- a/TimePlan.xlsx
+++ b/TimePlan.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Erweiterung</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t xml:space="preserve">Nicht-mischbare löschen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zutat doppelt</t>
   </si>
 </sst>
 </file>
@@ -653,12 +656,16 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1.25</v>
+      </c>
       <c r="C5" s="1"/>
       <c r="E5">
         <f>SUM(B5:C5)</f>
-        <v>0</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="6">

</xml_diff>